<commit_message>
Change graphics for results 6 end
</commit_message>
<xml_diff>
--- a/results/result_6_end.xlsx
+++ b/results/result_6_end.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PythonProjects\CalculateGraphs01\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{981D9FFF-CF6A-4995-9C88-B981CFADC9F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B37EE88-5BDA-4AC4-9E22-8F86A1130BC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="14016" xr2:uid="{0B45DCE8-D269-4F08-A321-ADD33B383C7B}"/>
   </bookViews>
@@ -643,6 +643,980 @@
           </c:marker>
           <c:val>
             <c:numRef>
+              <c:f>result_6_end!$A$1:$AD$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>2.3449419999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.076702E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3880760000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.61582594999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.0077940000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.2802360000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.6565299999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.2117099999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.3101099999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.8939109999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.2163429999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.3893700000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.6820080000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.20818627000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.3629640000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.791821E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.7931129999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.307851E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9.7009899999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.7538750000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.513893E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.6769230000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.127527E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.10128972999999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8.8391800000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.7184409999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>9.1903999999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.029473E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4CC7-4871-A0A8-010ED03B1419}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>result_6_end!$A$2:$AD$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>4.41305E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.59024414999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.4606980000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0612150000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.89573E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.13984505</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.4769500000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.8368929999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.6311299999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.4328059999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.5176600000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.2117099999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.9025100000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.12985E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.5490040000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.13111706000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.7116609999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.552071E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.019176E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.6535600000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.1297449999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9.3801600000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.9460459999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9.7391389999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>7.9651600000000006E-3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>9.6794900000000007E-3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.0995779999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>8.9143899999999995E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4CC7-4871-A0A8-010ED03B1419}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>result_6_end!$A$3:$AD$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>4.41305E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.59024414999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.4606980000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0612150000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.89573E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.13984505</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.4769500000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.8368929999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.6311299999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.4328059999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.5176600000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.2117099999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.9025100000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.12985E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.5490040000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.13111706000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.7116609999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.552071E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.019176E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.6535600000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.1297449999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9.3801600000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.9460459999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9.7391389999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>7.9651600000000006E-3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>9.6794900000000007E-3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.0995779999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>8.9143899999999995E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4CC7-4871-A0A8-010ED03B1419}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>result_6_end!$A$4:$AD$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>4.41305E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.59024414999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.4606980000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0612150000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.89573E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.13984505</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.4769500000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.8368929999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.6311299999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.4328059999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.5176600000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.2117099999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.9025100000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.12985E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.5490040000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.13111706000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.7116609999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.552071E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.019176E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.6535600000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.1297449999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9.3801600000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.9460459999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9.7391389999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>7.9651600000000006E-3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>9.6794900000000007E-3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.0995779999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>8.9143899999999995E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-4CC7-4871-A0A8-010ED03B1419}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>result_6_end!$A$5:$AD$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>9.3005699999999993E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.46228E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.197024E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.6450799999999994E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.7616749999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5744930000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.619821E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5176600000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.2117099999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.42479E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.6049360000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.3269199999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.16263369999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.3889959999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.6328510000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.0896399999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.6509960000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.1306700000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.10394829999999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.4384630000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>6.2512499999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.2574739999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.1451340000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.518478E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5.1436900000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>6.0601200000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.7192899999999999E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-4CC7-4871-A0A8-010ED03B1419}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>result_6_end!$A$6:$AD$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>1.0613340000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.3005699999999993E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.46228E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.197024E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.6450799999999994E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.7616749999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.5744930000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.619821E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.5176600000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.2117099999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.42479E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.6049360000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.3269199999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.16263369999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.3889959999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.6328510000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.0896399999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.6509960000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.1306700000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.10394829999999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.4384630000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>6.2512499999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.2574739999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.1451340000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.518478E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5.1436900000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>6.0601200000000001E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-4CC7-4871-A0A8-010ED03B1419}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>result_6_end!$A$7:$AD$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>1.218032E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9307959999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.108119E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.3358700000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.249902E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5583100000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0613340000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.3005699999999993E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.46228E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.197024E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.6450799999999994E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.7616749999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.5744930000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.619821E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.5176600000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.2117099999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.42479E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.6049360000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.3269199999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.16263369999999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.3889959999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.6328510000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.0896399999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.6509960000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.1306700000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.10394829999999999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.4384630000000001E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-4CC7-4871-A0A8-010ED03B1419}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>result_6_end!$A$8:$AD$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>5.249902E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5583100000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0613340000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.3005699999999993E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.46228E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.197024E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.6450799999999994E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.7616749999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.5744930000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.619821E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.5176600000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.2117099999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.42479E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.6049360000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.3269199999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.16263369999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.3889959999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.6328510000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.0896399999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.6509960000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.1306700000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.10394829999999999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.4384630000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6.2512499999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.2574739999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.1451340000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.518478E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-4CC7-4871-A0A8-010ED03B1419}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
               <c:f>result_6_end!$A$9:$AD$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -743,7 +1717,1120 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3CA5-4EC6-8F62-09412D63736E}"/>
+              <c16:uniqueId val="{00000008-4CC7-4871-A0A8-010ED03B1419}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>result_6_end!$A$10:$AD$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>6.2834299999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.12216856</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.2100699999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.8614549999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.056523E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.3581440000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.6565299999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.7660400000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.512201E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.8432090000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.2693309999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.25002E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.8554270000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.4850300000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.1804150000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.3400999999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.2610999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7.1133100000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.4160399999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.8123940000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.3146110000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5.3021300000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.8123940000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.3146110000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6.2512499999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.2574739999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7.0728600000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4.4320999999999996E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-4CC7-4871-A0A8-010ED03B1419}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>result_6_end!$A$11:$AD$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>0.17312105999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.4989759999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.3535700000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.211425E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.925338E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.8168430000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.8323199999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5176600000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.2117099999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.9025100000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.8471200000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.348689E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-4CC7-4871-A0A8-010ED03B1419}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>result_6_end!$A$12:$AD$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>3.3889959999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.6328510000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0896399999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.6509960000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.45686E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.3581440000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.6565299999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.2117099999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.3309400000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9.4133099999999994E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.925338E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.8168430000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.4323070000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.7757199999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.9407699999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8.9727399999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.7096099999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.533091E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.8218269999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.8482299999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.11830852</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>7.8401700000000005E-3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.315793E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.31043539999999997</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.7196989999999999E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-4CC7-4871-A0A8-010ED03B1419}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="12"/>
+          <c:order val="12"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>result_6_end!$A$13:$AD$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>3.3889959999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.6328510000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.94093E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.047758E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.3801600000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.8168430000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.8323199999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5176600000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.180379E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.1040570000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.5912699999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.7375100000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.532765E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9.755672E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.1627990000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.2219099999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9.748822E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.5734660000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>5.67565E-3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6.5373699999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.0204399999999999E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-4CC7-4871-A0A8-010ED03B1419}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="13"/>
+          <c:order val="13"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>result_6_end!$A$14:$AD$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>3.6328510000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.94093E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.047758E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.3801600000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.8168430000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.8323199999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.5176600000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.180379E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.1040570000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.5912699999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.7375100000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.532765E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.755672E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.1627990000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.2219099999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9.748822E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.5734660000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5.67565E-3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6.5373699999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3.0204399999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.11958972</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000D-4CC7-4871-A0A8-010ED03B1419}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="14"/>
+          <c:order val="14"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>result_6_end!$A$15:$AD$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>3.3889959999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.6328510000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0896399999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.6509960000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.45686E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.3581440000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.6565299999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.2117099999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.3309400000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9.4133099999999994E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.925338E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.8168430000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.4323070000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.7757199999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.9407699999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8.9727399999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.7096099999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.533091E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.8218269999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.8482299999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.11830852</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>7.8401700000000005E-3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.315793E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.31043539999999997</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.7196989999999999E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000E-4CC7-4871-A0A8-010ED03B1419}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="15"/>
+          <c:order val="15"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>result_6_end!$A$16:$AD$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>3.3889959999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.6328510000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.94093E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.047758E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.3801600000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.8168430000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.8323199999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5176600000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.180379E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.1040570000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.5912699999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.7375100000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.532765E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9.755672E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.1627990000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.2219099999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9.748822E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.5734660000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>5.67565E-3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6.5373699999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.0204399999999999E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000F-4CC7-4871-A0A8-010ED03B1419}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="16"/>
+          <c:order val="16"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>result_6_end!$A$17:$AD$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>3.3889959999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.6328510000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0896399999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.6509960000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.45686E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.3581440000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.6565299999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.2117099999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.3309400000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9.4133099999999994E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.925338E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.8168430000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.4323070000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.7757199999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.9407699999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8.9727399999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.7096099999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.533091E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.8218269999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.8482299999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.11830852</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>7.8401700000000005E-3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.315793E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.31043539999999997</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.7196989999999999E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000010-4CC7-4871-A0A8-010ED03B1419}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="17"/>
+          <c:order val="17"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>result_6_end!$A$18:$AD$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>3.3889959999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.6328510000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.94093E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.047758E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.3801600000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.8168430000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.8323199999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5176600000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.17834E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.180379E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.1040570000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.5912699999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.7375100000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.532765E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9.755672E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.1627990000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.2219099999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9.748822E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.5734660000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>5.67565E-3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6.5373699999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.0204399999999999E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000011-4CC7-4871-A0A8-010ED03B1419}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -756,11 +2843,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="968977824"/>
-        <c:axId val="968974944"/>
+        <c:axId val="1804383"/>
+        <c:axId val="1806303"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="968977824"/>
+        <c:axId val="1804383"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -802,7 +2889,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="968974944"/>
+        <c:crossAx val="1806303"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -810,7 +2897,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="968974944"/>
+        <c:axId val="1806303"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -861,7 +2948,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="968977824"/>
+        <c:crossAx val="1804383"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -873,6 +2960,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -984,99 +3102,99 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>result_6_end!$A$4:$AD$4</c:f>
+              <c:f>result_6_end!$A$19:$AD$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>4.41305E-3</c:v>
+                  <c:v>3.6652209999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.59024414999999997</c:v>
+                  <c:v>0.13079957</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.4606980000000001E-2</c:v>
+                  <c:v>1.017621E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0612150000000001E-2</c:v>
+                  <c:v>5.4755570000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.89573E-3</c:v>
+                  <c:v>1.644731E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.13984505</c:v>
+                  <c:v>6.511981E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.4769500000000004E-3</c:v>
+                  <c:v>2.0021230000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.8368929999999999E-2</c:v>
+                  <c:v>9.5588300000000008E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.6311299999999998E-3</c:v>
+                  <c:v>6.1532399999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.4328059999999996E-2</c:v>
+                  <c:v>2.003777E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.5176600000000001E-3</c:v>
+                  <c:v>6.0029599999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.17834E-3</c:v>
+                  <c:v>1.194167E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.17834E-3</c:v>
+                  <c:v>6.6762000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.2117099999999996E-3</c:v>
+                  <c:v>7.8755600000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.9025100000000001E-3</c:v>
+                  <c:v>8.8054899999999992E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.12985E-3</c:v>
+                  <c:v>2.869445E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4.5490040000000002E-2</c:v>
+                  <c:v>4.2232079999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.13111706000000001</c:v>
+                  <c:v>4.0294249999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.7116609999999999E-2</c:v>
+                  <c:v>2.2211789999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.552071E-2</c:v>
+                  <c:v>1.9906770000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.019176E-2</c:v>
+                  <c:v>2.9695639999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.6535600000000001E-3</c:v>
+                  <c:v>2.2211809999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.1297449999999999E-2</c:v>
+                  <c:v>3.9339810000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>9.3801600000000002E-3</c:v>
+                  <c:v>3.1470459999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>4.9460459999999998E-2</c:v>
+                  <c:v>3.1742630000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>9.7391389999999994E-2</c:v>
+                  <c:v>5.3513329999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>7.9651600000000006E-3</c:v>
+                  <c:v>9.2183899999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>9.6794900000000007E-3</c:v>
+                  <c:v>1.496637E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.0995779999999999E-2</c:v>
+                  <c:v>6.8379209999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>8.9143899999999995E-3</c:v>
+                  <c:v>2.491925E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1084,7 +3202,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-B421-4169-A8B1-DFF355620141}"/>
+              <c16:uniqueId val="{00000000-E628-4011-A5D5-7AC6AD26EC1D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1097,11 +3215,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1000779168"/>
-        <c:axId val="1000778208"/>
+        <c:axId val="1809663"/>
+        <c:axId val="1800543"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1000779168"/>
+        <c:axId val="1809663"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1143,7 +3261,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1000778208"/>
+        <c:crossAx val="1800543"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1151,7 +3269,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1000778208"/>
+        <c:axId val="1800543"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1202,689 +3320,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1000779168"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="ru-RU"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>result_6_end!$A$7:$AD$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
-                <c:pt idx="0">
-                  <c:v>1.218032E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.9307959999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.108119E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8.3358700000000004E-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.249902E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.5583100000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.0613340000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9.3005699999999993E-3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9.46228E-3</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.197024E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>8.6450799999999994E-3</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2.7616749999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.5744930000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2.619821E-2</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>3.5176600000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>5.17834E-3</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>5.17834E-3</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>5.17834E-3</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>4.2117099999999996E-3</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>3.42479E-3</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2.6049360000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>4.3269199999999997E-3</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.16263369999999999</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>3.3889959999999997E-2</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>3.6328510000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>2.0896399999999998E-3</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>3.6509960000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>4.1306700000000003E-3</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0.10394829999999999</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>2.4384630000000001E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-CE3E-4897-9D67-1751B24D69A2}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="1015318416"/>
-        <c:axId val="1015318896"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="1015318416"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1015318896"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1015318896"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1015318416"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="ru-RU"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>result_6_end!$A$19:$AD$19</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
-                <c:pt idx="0">
-                  <c:v>3.6652209999999998E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.13079957</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.017621E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.4755570000000003E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.644731E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6.511981E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.0021230000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9.5588300000000008E-3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>6.1532399999999999E-3</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.003777E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6.0029599999999999E-3</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.194167E-2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>6.6762000000000002E-3</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>7.8755600000000002E-3</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>8.8054899999999992E-3</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2.869445E-2</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>4.2232079999999998E-2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>4.0294249999999997E-2</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>2.2211789999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1.9906770000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2.9695639999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>2.2211809999999998E-2</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>3.9339810000000003E-2</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>3.1470459999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>3.1742630000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>5.3513329999999998E-2</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>9.2183899999999999E-3</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>1.496637E-2</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>6.8379209999999996E-2</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>2.491925E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-A7F4-4B8F-BECF-3FF36FEB0B53}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="968980496"/>
-        <c:axId val="968979536"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="968980496"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="968979536"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="968979536"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="968980496"/>
+        <c:crossAx val="1809663"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1981,86 +3417,6 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3132,1059 +4488,27 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>281940</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>34290</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>68580</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>87630</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>586740</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>34290</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>137160</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Диаграмма 2">
+        <xdr:cNvPr id="6" name="Диаграмма 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC1999A4-3FA1-FAA2-EB9D-50A11AF9F473}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE7622F1-41F1-987F-5291-C6AD6E8E190F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4204,23 +4528,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>601980</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>26670</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>259080</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>297180</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>26670</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>563880</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Диаграмма 3">
+        <xdr:cNvPr id="7" name="Диаграмма 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{701C12B3-1246-6B23-CD1C-9EE92A4A8608}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8A2C174-0488-10F6-9CA8-2E183EDFBDBB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4233,78 +4557,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>358140</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>3810</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>53340</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>3810</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Диаграмма 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C11A1F5-B88C-F99E-5799-A9071014206C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>464820</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>53340</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Диаграмма 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BCD8039-A838-C122-4AD3-0DCDB33ADE14}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4632,8 +4884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C2FF872-7BBC-4908-995D-02D3DC808D91}">
   <dimension ref="A1:AD19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="Q38" sqref="Q38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>